<commit_message>
Added name validatiion and fixed frontend
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Sample_metadata_v3_8_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Sample_metadata_v3_8_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791A6E88-41E0-104C-B6CB-C7D090BD2AC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4928CE64-130F-6840-8D01-45B3547D5153}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15940" xr2:uid="{82938438-56AF-234A-A3B8-D78369EC91CE}"/>
   </bookViews>
@@ -70,12 +70,6 @@
     <t>CONTAINER4METADATA</t>
   </si>
   <si>
-    <t>MetadataName1</t>
-  </si>
-  <si>
-    <t>MetadataName2</t>
-  </si>
-  <si>
     <t>MetadataName3</t>
   </si>
   <si>
@@ -98,6 +92,12 @@
   </si>
   <si>
     <t>MetadataValue5</t>
+  </si>
+  <si>
+    <t>Metadata Name 1</t>
+  </si>
+  <si>
+    <t>Metadata Name 2</t>
   </si>
 </sst>
 </file>
@@ -564,9 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392F720A-4E7D-5248-A2A0-643EBDB15234}">
   <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -643,13 +641,13 @@
         <v>7</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -673,13 +671,13 @@
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -687,18 +685,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>